<commit_message>
Update TARJETA DE LIQUIDACION 2012.xlsx
</commit_message>
<xml_diff>
--- a/TARJETA PATAYPAMPA/TARJETA DE LIQUIDACION 2012.xlsx
+++ b/TARJETA PATAYPAMPA/TARJETA DE LIQUIDACION 2012.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUPERVISION2020\TARJETA PATAYPAMPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SUPERVISION2020\TARJETA PATAYPAMPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1357,87 +1357,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1462,15 +1381,6 @@
     <xf numFmtId="17" fontId="10" fillId="0" borderId="31" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="17" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1508,29 +1418,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="17" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1548,15 +1440,6 @@
     <xf numFmtId="4" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="17" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1584,6 +1467,123 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3581,13 +3581,13 @@
       <c r="AA10" s="19"/>
     </row>
     <row r="11" spans="2:27" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="83"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="126"/>
       <c r="G11" s="21" t="s">
         <v>40</v>
       </c>
@@ -4414,7 +4414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
@@ -4427,28 +4427,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
     </row>
     <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -4601,43 +4601,43 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="88" t="s">
+      <c r="C8" s="130"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="91" t="s">
+      <c r="G8" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="92" t="s">
+      <c r="H8" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="93"/>
-      <c r="P8" s="93"/>
+      <c r="I8" s="136"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="136"/>
+      <c r="L8" s="136"/>
+      <c r="M8" s="136"/>
+      <c r="N8" s="136"/>
+      <c r="O8" s="136"/>
+      <c r="P8" s="136"/>
       <c r="Q8" s="48"/>
       <c r="R8" s="48"/>
       <c r="S8" s="48"/>
-      <c r="T8" s="91" t="s">
+      <c r="T8" s="134" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="86"/>
+      <c r="A9" s="129"/>
       <c r="B9" s="12" t="s">
         <v>16</v>
       </c>
@@ -4647,9 +4647,9 @@
       <c r="D9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="89"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="86"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="129"/>
       <c r="H9" s="13" t="s">
         <v>19</v>
       </c>
@@ -4686,7 +4686,7 @@
       <c r="S9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="86"/>
+      <c r="T9" s="129"/>
     </row>
     <row r="10" spans="1:20" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="52">
@@ -4868,7 +4868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -4884,34 +4884,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77"/>
@@ -4927,19 +4927,19 @@
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="127" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -4981,16 +4981,16 @@
       <c r="C7" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
     </row>
     <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -5000,16 +5000,16 @@
       <c r="C8" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="139" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139"/>
     </row>
     <row r="9" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -5046,34 +5046,34 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="88" t="s">
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="92" t="s">
+      <c r="H11" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="93"/>
-      <c r="J11" s="93"/>
-      <c r="K11" s="91" t="s">
+      <c r="I11" s="136"/>
+      <c r="J11" s="136"/>
+      <c r="K11" s="134" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
+      <c r="A12" s="129"/>
       <c r="B12" s="47" t="s">
         <v>16</v>
       </c>
@@ -5083,9 +5083,9 @@
       <c r="D12" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="89"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="86"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="129"/>
       <c r="H12" s="13" t="s">
         <v>19</v>
       </c>
@@ -5095,13 +5095,13 @@
       <c r="J12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="86"/>
+      <c r="K12" s="129"/>
     </row>
     <row r="13" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="52">
         <v>1</v>
       </c>
-      <c r="B13" s="117">
+      <c r="B13" s="90">
         <v>41620</v>
       </c>
       <c r="C13" s="49" t="s">
@@ -5136,31 +5136,31 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="119"/>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="121">
+      <c r="B14" s="141"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="141"/>
+      <c r="F14" s="142"/>
+      <c r="G14" s="91">
         <f>SUM(G13)</f>
         <v>410930.5</v>
       </c>
-      <c r="H14" s="121">
+      <c r="H14" s="91">
         <f>SUM(H13)</f>
         <v>148489</v>
       </c>
-      <c r="I14" s="121">
+      <c r="I14" s="91">
         <f t="shared" ref="I14:J14" si="0">SUM(I13)</f>
         <v>230561.5</v>
       </c>
-      <c r="J14" s="121">
+      <c r="J14" s="91">
         <f t="shared" si="0"/>
         <v>31880</v>
       </c>
-      <c r="K14" s="122"/>
+      <c r="K14" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -5188,7 +5188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -5201,34 +5201,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77"/>
@@ -5244,19 +5244,19 @@
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="127" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -5298,16 +5298,16 @@
       <c r="C7" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
     </row>
     <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -5317,16 +5317,16 @@
       <c r="C8" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="139" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139"/>
     </row>
     <row r="9" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -5363,32 +5363,32 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="99"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="88" t="s">
+      <c r="C11" s="150"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="103"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="105"/>
-      <c r="K11" s="91" t="s">
+      <c r="H11" s="144"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="146"/>
+      <c r="K11" s="134" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="97"/>
+      <c r="A12" s="148"/>
       <c r="B12" s="64" t="s">
         <v>16</v>
       </c>
@@ -5398,9 +5398,9 @@
       <c r="D12" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="102"/>
+      <c r="E12" s="152"/>
+      <c r="F12" s="152"/>
+      <c r="G12" s="143"/>
       <c r="H12" s="65" t="s">
         <v>24</v>
       </c>
@@ -5410,13 +5410,13 @@
       <c r="J12" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="102"/>
+      <c r="K12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="66">
         <v>2</v>
       </c>
-      <c r="B13" s="117">
+      <c r="B13" s="90">
         <v>41620</v>
       </c>
       <c r="C13" s="49" t="s">
@@ -5425,7 +5425,7 @@
       <c r="D13" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="124">
+      <c r="E13" s="94">
         <v>10975</v>
       </c>
       <c r="F13" s="70" t="s">
@@ -5446,39 +5446,44 @@
         <f>1204-1204</f>
         <v>0</v>
       </c>
-      <c r="K13" s="108" t="s">
+      <c r="K13" s="81" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="119"/>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="141"/>
-      <c r="G14" s="142">
+      <c r="B14" s="141"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="141"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="106">
         <f>SUM(G13)</f>
         <v>6000</v>
       </c>
-      <c r="H14" s="142">
+      <c r="H14" s="106">
         <f t="shared" ref="H14:J14" si="0">SUM(H13)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="142">
+      <c r="I14" s="106">
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
-      <c r="J14" s="142">
+      <c r="J14" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="123"/>
+      <c r="K14" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="K11:K12"/>
@@ -5487,11 +5492,6 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="62" orientation="landscape" r:id="rId1"/>
@@ -5502,7 +5502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="130" zoomScaleNormal="70" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -5515,34 +5515,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77"/>
@@ -5558,19 +5558,19 @@
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="127" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -5612,14 +5612,14 @@
       <c r="C7" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
       <c r="J7" s="80"/>
       <c r="K7" s="80"/>
     </row>
@@ -5631,75 +5631,75 @@
       <c r="C8" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="139" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
       <c r="J8" s="80"/>
       <c r="K8" s="80"/>
     </row>
     <row r="9" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="110"/>
-      <c r="C9" s="111" t="s">
+      <c r="B9" s="83"/>
+      <c r="C9" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="110" t="s">
+      <c r="D9" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="115"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="112"/>
-      <c r="I10" s="113">
+      <c r="A10" s="88"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="86">
         <v>2012</v>
       </c>
-      <c r="J10" s="114"/>
+      <c r="J10" s="87"/>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="88" t="s">
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="134" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="74"/>
-      <c r="I11" s="91" t="s">
+      <c r="I11" s="134" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="102"/>
+      <c r="A12" s="143"/>
       <c r="B12" s="64" t="s">
         <v>16</v>
       </c>
@@ -5709,65 +5709,70 @@
       <c r="D12" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="106"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="102"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="152"/>
+      <c r="G12" s="143"/>
       <c r="H12" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="102"/>
+      <c r="I12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="125">
+      <c r="A13" s="95">
         <v>1</v>
       </c>
-      <c r="B13" s="126">
+      <c r="B13" s="96">
         <v>41620</v>
       </c>
-      <c r="C13" s="127" t="s">
+      <c r="C13" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="128" t="s">
+      <c r="D13" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="129" t="s">
+      <c r="E13" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="130">
+      <c r="F13" s="100">
         <v>5739</v>
       </c>
-      <c r="G13" s="131">
+      <c r="G13" s="101">
         <f>SUM(H13:H13)</f>
         <v>12316</v>
       </c>
-      <c r="H13" s="132">
+      <c r="H13" s="102">
         <v>12316</v>
       </c>
-      <c r="I13" s="133" t="s">
+      <c r="I13" s="103" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="136" t="s">
+      <c r="A14" s="153" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="137"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="139">
+      <c r="B14" s="154"/>
+      <c r="C14" s="154"/>
+      <c r="D14" s="154"/>
+      <c r="E14" s="154"/>
+      <c r="F14" s="155"/>
+      <c r="G14" s="104">
         <f>SUM(G13)</f>
         <v>12316</v>
       </c>
-      <c r="H14" s="139">
+      <c r="H14" s="104">
         <f t="shared" ref="H14" si="0">SUM(H13)</f>
         <v>12316</v>
       </c>
-      <c r="I14" s="140"/>
+      <c r="I14" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="A14:F14"/>
@@ -5775,11 +5780,6 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
@@ -5793,7 +5793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="70" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
@@ -5807,34 +5807,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77"/>
@@ -5850,19 +5850,19 @@
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="127" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -5904,15 +5904,15 @@
       <c r="C7" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
       <c r="K7" s="80"/>
     </row>
     <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5923,34 +5923,34 @@
       <c r="C8" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="139" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
       <c r="K8" s="80"/>
     </row>
     <row r="9" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="110"/>
-      <c r="C9" s="111" t="s">
+      <c r="B9" s="83"/>
+      <c r="C9" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="110" t="s">
+      <c r="D9" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5968,31 +5968,31 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="88" t="s">
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="91" t="s">
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="134" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="102"/>
+      <c r="A12" s="143"/>
       <c r="B12" s="64" t="s">
         <v>16</v>
       </c>
@@ -6002,34 +6002,34 @@
       <c r="D12" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="106"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="102"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="152"/>
+      <c r="G12" s="143"/>
       <c r="H12" s="65" t="s">
         <v>22</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="102"/>
+      <c r="J12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="143">
+      <c r="A13" s="107">
         <v>1</v>
       </c>
-      <c r="B13" s="126">
+      <c r="B13" s="96">
         <v>41620</v>
       </c>
-      <c r="C13" s="127" t="s">
+      <c r="C13" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="128" t="s">
+      <c r="D13" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="129" t="s">
+      <c r="E13" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="144">
+      <c r="F13" s="108">
         <v>5739</v>
       </c>
       <c r="G13" s="67">
@@ -6042,48 +6042,48 @@
       <c r="I13" s="67">
         <v>41166</v>
       </c>
-      <c r="J13" s="145" t="s">
+      <c r="J13" s="109" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="134" t="s">
+      <c r="A14" s="157" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="135"/>
-      <c r="C14" s="135"/>
-      <c r="D14" s="135"/>
-      <c r="E14" s="135"/>
-      <c r="F14" s="135"/>
-      <c r="G14" s="146">
+      <c r="B14" s="158"/>
+      <c r="C14" s="158"/>
+      <c r="D14" s="158"/>
+      <c r="E14" s="158"/>
+      <c r="F14" s="158"/>
+      <c r="G14" s="110">
         <f>SUM(G13)</f>
         <v>91166</v>
       </c>
-      <c r="H14" s="147">
+      <c r="H14" s="111">
         <f t="shared" ref="H14:I14" si="0">SUM(H13)</f>
         <v>50000</v>
       </c>
-      <c r="I14" s="146">
+      <c r="I14" s="110">
         <f t="shared" si="0"/>
         <v>41166</v>
       </c>
-      <c r="J14" s="148"/>
+      <c r="J14" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="D8:J8"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="69" orientation="landscape" r:id="rId1"/>
@@ -6097,7 +6097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="78" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -6110,34 +6110,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77"/>
@@ -6153,19 +6153,19 @@
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -6207,16 +6207,16 @@
       <c r="C7" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
     </row>
     <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -6226,34 +6226,34 @@
       <c r="C8" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="139" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139"/>
     </row>
     <row r="9" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="110"/>
-      <c r="C9" s="111" t="s">
+      <c r="B9" s="83"/>
+      <c r="C9" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="110" t="s">
+      <c r="D9" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
       <c r="K9" s="8"/>
     </row>
     <row r="11" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -6272,34 +6272,34 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="88" t="s">
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="88" t="s">
+      <c r="F12" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="91" t="s">
+      <c r="G12" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="93" t="s">
+      <c r="H12" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="93"/>
-      <c r="J12" s="107"/>
-      <c r="K12" s="91" t="s">
+      <c r="I12" s="136"/>
+      <c r="J12" s="162"/>
+      <c r="K12" s="134" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="102"/>
+      <c r="A13" s="143"/>
       <c r="B13" s="64" t="s">
         <v>16</v>
       </c>
@@ -6309,9 +6309,9 @@
       <c r="D13" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="106"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="102"/>
+      <c r="E13" s="156"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="143"/>
       <c r="H13" s="65" t="s">
         <v>28</v>
       </c>
@@ -6321,70 +6321,70 @@
       <c r="J13" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="102"/>
+      <c r="K13" s="143"/>
     </row>
     <row r="14" spans="1:11" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="155">
+      <c r="A14" s="116">
         <v>1</v>
       </c>
-      <c r="B14" s="117">
+      <c r="B14" s="90">
         <v>41620</v>
       </c>
-      <c r="C14" s="156" t="s">
+      <c r="C14" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="157" t="s">
+      <c r="D14" s="118" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="158" t="s">
+      <c r="E14" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="159" t="s">
+      <c r="F14" s="120" t="s">
         <v>110</v>
       </c>
-      <c r="G14" s="160">
+      <c r="G14" s="121">
         <f>SUM(H14:J14)</f>
         <v>2493</v>
       </c>
-      <c r="H14" s="161"/>
-      <c r="I14" s="160">
+      <c r="H14" s="122"/>
+      <c r="I14" s="121">
         <f>1896-596</f>
         <v>1300</v>
       </c>
-      <c r="J14" s="160">
+      <c r="J14" s="121">
         <f>1897-704</f>
         <v>1193</v>
       </c>
-      <c r="K14" s="162" t="s">
+      <c r="K14" s="123" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="149" t="s">
+      <c r="A15" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="150"/>
-      <c r="C15" s="150"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="150"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="152">
+      <c r="B15" s="160"/>
+      <c r="C15" s="160"/>
+      <c r="D15" s="160"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="161"/>
+      <c r="G15" s="113">
         <f>SUM(G14:G14)</f>
         <v>2493</v>
       </c>
-      <c r="H15" s="154">
+      <c r="H15" s="115">
         <f>SUM(H14:H14)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="152">
+      <c r="I15" s="113">
         <f>SUM(I14:I14)</f>
         <v>1300</v>
       </c>
-      <c r="J15" s="154">
+      <c r="J15" s="115">
         <f>SUM(J14:J14)</f>
         <v>1193</v>
       </c>
-      <c r="K15" s="153"/>
+      <c r="K15" s="114"/>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" s="56"/>
@@ -6396,11 +6396,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="A12:A13"/>
@@ -6409,6 +6404,11 @@
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:J12"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="59" orientation="landscape" r:id="rId1"/>

</xml_diff>